<commit_message>
Register user form added, Offices menu added
</commit_message>
<xml_diff>
--- a/items_management/static/reports/items_report.xlsx
+++ b/items_management/static/reports/items_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1569,58 +1569,6 @@
         <v>0</v>
       </c>
       <c r="N24" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>21</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Alfa-Romeo</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>12-00-01</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>12423</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" t="n">
-        <v>12423</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>В работе</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>23423</v>
-      </c>
-      <c r="J25" t="n">
-        <v>-1</v>
-      </c>
-      <c r="K25" t="n">
-        <v>-23423</v>
-      </c>
-      <c r="L25" t="n">
-        <v>1</v>
-      </c>
-      <c r="M25" t="n">
-        <v>23423</v>
-      </c>
-      <c r="N25" t="inlineStr">
         <is>
           <t>admin</t>
         </is>

</xml_diff>